<commit_message>
write about purpose of the research
</commit_message>
<xml_diff>
--- a/literature/Google Trend.xlsx
+++ b/literature/Google Trend.xlsx
@@ -123,6 +123,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -637,6 +644,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1151,6 +1168,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1640,11 +1664,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2146148312"/>
-        <c:axId val="2104496232"/>
+        <c:axId val="-2114350680"/>
+        <c:axId val="-2118501304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2146148312"/>
+        <c:axId val="-2114350680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +1698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104496232"/>
+        <c:crossAx val="-2118501304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1683,7 +1707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104496232"/>
+        <c:axId val="-2118501304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1706,7 +1730,6 @@
                   <a:rPr lang="ja-JP" altLang="en-US"/>
                   <a:t>　</a:t>
                 </a:r>
-                <a:endParaRPr lang="ja-JP" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1717,7 +1740,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146148312"/>
+        <c:crossAx val="-2114350680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1731,6 +1754,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1750,7 +1778,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
+      <xdr:colOff>787400</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2099,7 +2127,7 @@
   <dimension ref="A1:J158"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>